<commit_message>
Add a single sample excel file
</commit_message>
<xml_diff>
--- a/test_data/single.xlsx
+++ b/test_data/single.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t xml:space="preserve">Ti-6Al-4V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WORKSHEET: ABC123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P:Temperature</t>
   </si>
   <si>
     <t xml:space="preserve">P:Label</t>
@@ -211,7 +217,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -296,10 +302,28 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>118.150523470234</v>
-      </c>
-    </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>135.978543903077</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="e">
+        <f aca="false">===</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>400</v>
+      </c>
+    </row>
     <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -342,19 +366,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="ALS1" s="0"/>
       <c r="ALT1" s="0"/>
@@ -380,22 +404,22 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -438,10 +462,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,13 +473,13 @@
         <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>